<commit_message>
change for larger matrix
</commit_message>
<xml_diff>
--- a/CF/data.xlsx
+++ b/CF/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b3f4bae0c2687e0/Documents/GitHub/Sheminar-py-server/CF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55343A4C-E922-4791-87E0-00FA98E8127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EB9AAFAC-69AF-4AE2-B065-63C4F1FA3F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FCA49B-65DE-48BA-8632-9F330C2DFD56}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0A323DD1-B6D1-43A5-B75B-4E25607BDF68}"/>
   </bookViews>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF84092-840D-40E6-B1A2-8A18FACE79B2}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>